<commit_message>
Added Account Creation Test and corresponding changes
</commit_message>
<xml_diff>
--- a/MyStoreProject/TestData/testData.xlsx
+++ b/MyStoreProject/TestData/testData.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16125" windowHeight="2505" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14085" windowHeight="2730" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="NewAccount" sheetId="2" r:id="rId2"/>
     <sheet name="TestCases" sheetId="3" r:id="rId3"/>
+    <sheet name="AccountCreationData" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>username</t>
   </si>
@@ -39,14 +40,125 @@
     <t>eMail</t>
   </si>
   <si>
-    <t>lakshmi.cbe@hotmail.com</t>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>SetPassword</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>OptinOffer</t>
+  </si>
+  <si>
+    <t>Newsletter</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Lakshmi</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Jasu@mailinator.com</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>Jaswanthika</t>
+  </si>
+  <si>
+    <t>Jasu@31</t>
+  </si>
+  <si>
+    <t>Sathish@mailinator.com</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>Sathish</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>sathish@14</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>lakshmi@mailinator.com</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>lakshmi6@mailinator.com</t>
+  </si>
+  <si>
+    <t>Jasu6@mailinator.com</t>
+  </si>
+  <si>
+    <t>Sathish6@mailinator.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +180,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -77,7 +197,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,12 +205,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -99,6 +234,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -160,7 +298,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -195,7 +333,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -449,10 +587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,12 +602,24 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -487,4 +637,164 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="E4" r:id="rId5"/>
+    <hyperlink ref="A2" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+</worksheet>
 </file>
</xml_diff>